<commit_message>
updated spreadsheet, and generate programme
</commit_message>
<xml_diff>
--- a/TESimplespreadsheet.xlsx
+++ b/TESimplespreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="154">
   <si>
     <t xml:space="preserve">back </t>
   </si>
@@ -463,9 +463,6 @@
   </si>
   <si>
     <t>editorial</t>
-  </si>
-  <si>
-    <t>KILL? Check usage</t>
   </si>
   <si>
     <t>associated with term?</t>
@@ -640,7 +637,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -649,8 +646,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -720,7 +718,7 @@
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:G134">
-    <sortCondition ref="F1:F134"/>
+    <sortCondition ref="A1:A134"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="element"/>
@@ -1060,8 +1058,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1096,7 +1094,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>54</v>
@@ -1105,21 +1103,18 @@
         <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>128</v>
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>82</v>
@@ -1131,21 +1126,21 @@
         <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -1155,48 +1150,51 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>54</v>
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
         <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>54</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>128</v>
+        <v>110</v>
+      </c>
+      <c r="G6" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>87</v>
+      <c r="A7" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
@@ -1207,36 +1205,30 @@
       <c r="D7" t="s">
         <v>54</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>128</v>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>147</v>
+        <v>54</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
@@ -1244,138 +1236,126 @@
       <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
+      <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>82</v>
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>147</v>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>82</v>
       </c>
-      <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>147</v>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F12" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>54</v>
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" t="s">
-        <v>147</v>
+        <v>47</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>138</v>
+      <c r="A14" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>82</v>
       </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
       <c r="E15" t="s">
         <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C16" t="s">
@@ -1388,15 +1368,15 @@
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
+      <c r="A17" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C17" t="s">
         <v>82</v>
@@ -1405,15 +1385,15 @@
         <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>54</v>
@@ -1428,12 +1408,12 @@
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>54</v>
@@ -1441,51 +1421,53 @@
       <c r="C19" t="s">
         <v>82</v>
       </c>
-      <c r="D19" t="s">
-        <v>47</v>
+      <c r="D19" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
-      </c>
-      <c r="F19" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
-      </c>
-      <c r="F20" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>54</v>
@@ -1493,56 +1475,56 @@
       <c r="C22" t="s">
         <v>82</v>
       </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="D22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>84</v>
-      </c>
-    </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="1" t="s">
-        <v>114</v>
+      <c r="A25" t="s">
+        <v>92</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
@@ -1550,87 +1532,81 @@
       <c r="C25" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="s">
         <v>54</v>
       </c>
       <c r="E25" t="s">
         <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
+        <v>110</v>
+      </c>
+      <c r="G25" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" t="s">
-        <v>146</v>
-      </c>
-      <c r="G26" t="s">
-        <v>150</v>
+        <v>83</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>137</v>
+      <c r="A27" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
         <v>82</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>146</v>
-      </c>
-      <c r="G27" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>82</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>47</v>
+        <v>47</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>151</v>
-      </c>
-      <c r="G28" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="A29" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C29" t="s">
@@ -1639,36 +1615,30 @@
       <c r="D29" t="s">
         <v>47</v>
       </c>
-      <c r="E29" t="s">
-        <v>54</v>
-      </c>
       <c r="F29" t="s">
-        <v>151</v>
-      </c>
-      <c r="G29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>54</v>
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
       </c>
       <c r="C30" t="s">
         <v>82</v>
       </c>
+      <c r="D30" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="E30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" t="s">
-        <v>134</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="3" t="s">
-        <v>61</v>
+      <c r="A31" t="s">
+        <v>93</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>54</v>
@@ -1676,19 +1646,19 @@
       <c r="C31" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>54</v>
+      <c r="D31" t="s">
+        <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="3" t="s">
-        <v>57</v>
+      <c r="A32" t="s">
+        <v>94</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>54</v>
@@ -1697,13 +1667,13 @@
         <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:7" hidden="1">
@@ -1721,8 +1691,8 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="3" t="s">
-        <v>55</v>
+      <c r="A34" t="s">
+        <v>95</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>54</v>
@@ -1734,15 +1704,15 @@
         <v>54</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F34" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="6" t="s">
-        <v>118</v>
+      <c r="A35" t="s">
+        <v>96</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>54</v>
@@ -1751,62 +1721,53 @@
         <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
       </c>
       <c r="F35" t="s">
-        <v>110</v>
-      </c>
-      <c r="G35" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C36" t="s">
         <v>82</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" t="s">
         <v>47</v>
       </c>
       <c r="F36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G36" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>88</v>
+      <c r="A37" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
         <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F37" t="s">
-        <v>110</v>
-      </c>
-      <c r="G37" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:7" hidden="1">
@@ -1825,8 +1786,8 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>92</v>
+      <c r="A39" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="B39" t="s">
         <v>54</v>
@@ -1841,61 +1802,46 @@
         <v>47</v>
       </c>
       <c r="F39" t="s">
-        <v>110</v>
-      </c>
-      <c r="G39" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="6" t="s">
-        <v>99</v>
+      <c r="A40" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
         <v>82</v>
       </c>
-      <c r="D40" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" t="s">
-        <v>145</v>
+      <c r="D40" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="1" t="s">
-        <v>102</v>
+      <c r="A41" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" t="s">
-        <v>110</v>
-      </c>
-      <c r="G41" t="s">
-        <v>145</v>
+      <c r="D41" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="1" t="s">
-        <v>112</v>
+      <c r="A42" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B42" t="s">
         <v>54</v>
@@ -1903,24 +1849,18 @@
       <c r="C42" t="s">
         <v>82</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" t="s">
-        <v>110</v>
-      </c>
-      <c r="G42" t="s">
-        <v>145</v>
+      <c r="D42" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="A43" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C43" t="s">
@@ -1931,17 +1871,11 @@
       </c>
       <c r="E43" t="s">
         <v>47</v>
-      </c>
-      <c r="F43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G43" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B44" t="s">
         <v>54</v>
@@ -1949,7 +1883,7 @@
       <c r="C44" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" t="s">
         <v>54</v>
       </c>
       <c r="E44" t="s">
@@ -1964,7 +1898,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
         <v>54</v>
@@ -1972,42 +1906,33 @@
       <c r="C45" t="s">
         <v>82</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E45" t="s">
         <v>47</v>
       </c>
-      <c r="F45" t="s">
-        <v>110</v>
-      </c>
-      <c r="G45" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>54</v>
+      <c r="A46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
       </c>
       <c r="C46" t="s">
         <v>82</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E46" t="s">
         <v>47</v>
       </c>
-      <c r="F46" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" t="s">
-        <v>94</v>
+      <c r="A47" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>54</v>
@@ -2015,14 +1940,11 @@
       <c r="C47" t="s">
         <v>82</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E47" t="s">
         <v>47</v>
-      </c>
-      <c r="F47" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:7" hidden="1">
@@ -2037,7 +1959,7 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:6" hidden="1">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="3" t="s">
         <v>75</v>
       </c>
@@ -2049,9 +1971,9 @@
       </c>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>95</v>
+    <row r="50" spans="1:7">
+      <c r="A50" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>54</v>
@@ -2059,22 +1981,19 @@
       <c r="C50" t="s">
         <v>82</v>
       </c>
-      <c r="D50" t="s">
-        <v>54</v>
+      <c r="D50" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E50" t="s">
-        <v>47</v>
-      </c>
-      <c r="F50" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>54</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
       </c>
       <c r="C51" t="s">
         <v>82</v>
@@ -2082,14 +2001,14 @@
       <c r="D51" t="s">
         <v>47</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F51" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" hidden="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52" s="3" t="s">
         <v>69</v>
       </c>
@@ -2101,29 +2020,32 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" s="3" t="s">
+    <row r="53" spans="1:7">
+      <c r="A53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
         <v>54</v>
       </c>
       <c r="C53" t="s">
         <v>82</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E53" t="s">
         <v>47</v>
       </c>
       <c r="F53" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="6" t="s">
-        <v>103</v>
+        <v>110</v>
+      </c>
+      <c r="G53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="B54" t="s">
         <v>54</v>
@@ -2135,13 +2057,13 @@
         <v>47</v>
       </c>
       <c r="E54" t="s">
-        <v>47</v>
-      </c>
-      <c r="F54" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" hidden="1">
+        <v>54</v>
+      </c>
+      <c r="G54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
@@ -2153,9 +2075,9 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="4" t="s">
-        <v>123</v>
+    <row r="56" spans="1:7">
+      <c r="A56" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -2167,97 +2089,85 @@
         <v>47</v>
       </c>
       <c r="E56" t="s">
-        <v>47</v>
-      </c>
-      <c r="F56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E60" t="s">
+        <v>47</v>
+      </c>
+      <c r="F60" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C57" t="s">
-        <v>82</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E57" t="s">
-        <v>47</v>
-      </c>
-      <c r="F57" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" t="s">
-        <v>47</v>
-      </c>
-      <c r="C58" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" t="s">
-        <v>47</v>
-      </c>
-      <c r="C59" t="s">
-        <v>82</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F59" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" t="s">
-        <v>47</v>
-      </c>
-      <c r="C60" t="s">
-        <v>82</v>
-      </c>
-      <c r="D60" t="s">
-        <v>47</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F60" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:7">
       <c r="A61" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C61" t="s">
@@ -2269,33 +2179,25 @@
       <c r="E61" t="s">
         <v>47</v>
       </c>
-      <c r="F61" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C62" t="s">
         <v>82</v>
       </c>
-      <c r="D62" t="s">
-        <v>47</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F62" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="D62" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="7" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>47</v>
@@ -2303,21 +2205,16 @@
       <c r="C63" t="s">
         <v>82</v>
       </c>
-      <c r="D63" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E63" t="s">
-        <v>47</v>
-      </c>
-      <c r="F63" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="D63" t="s">
+        <v>47</v>
+      </c>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C64" t="s">
@@ -2326,51 +2223,37 @@
       <c r="D64" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F64" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C65" t="s">
         <v>82</v>
       </c>
-      <c r="D65" t="s">
-        <v>47</v>
-      </c>
-      <c r="E65" t="s">
-        <v>47</v>
-      </c>
-      <c r="F65" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="D65" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C66" t="s">
         <v>82</v>
       </c>
-      <c r="D66" t="s">
-        <v>47</v>
-      </c>
-      <c r="E66" t="s">
-        <v>47</v>
-      </c>
-      <c r="F66" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" hidden="1">
+      <c r="D66" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1">
       <c r="A67" s="7" t="s">
         <v>73</v>
       </c>
@@ -2382,27 +2265,24 @@
       </c>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" t="s">
-        <v>47</v>
+    <row r="68" spans="1:7">
+      <c r="A68" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C68" t="s">
         <v>82</v>
       </c>
-      <c r="D68" t="s">
-        <v>47</v>
+      <c r="D68" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E68" t="s">
-        <v>152</v>
-      </c>
-      <c r="F68" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" hidden="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" hidden="1">
       <c r="A69" s="7" t="s">
         <v>78</v>
       </c>
@@ -2414,43 +2294,49 @@
       </c>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70" s="3" t="s">
+    <row r="70" spans="1:7">
+      <c r="A70" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B70" t="s">
         <v>54</v>
       </c>
       <c r="C70" t="s">
         <v>82</v>
       </c>
-      <c r="D70" t="s">
-        <v>47</v>
+      <c r="D70" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>47</v>
+      </c>
+      <c r="F70" t="s">
+        <v>150</v>
+      </c>
+      <c r="G70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B71" t="s">
-        <v>54</v>
+        <v>42</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C71" t="s">
         <v>82</v>
       </c>
-      <c r="D71" t="s">
-        <v>54</v>
+      <c r="D71" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E71" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="7" t="s">
-        <v>90</v>
+    <row r="72" spans="1:7">
+      <c r="A72" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="B72" t="s">
         <v>54</v>
@@ -2464,25 +2350,31 @@
       <c r="E72" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" hidden="1">
+      <c r="F72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B73" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" t="s">
+        <v>54</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F73" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1">
       <c r="A74" s="5" t="s">
         <v>104</v>
       </c>
@@ -2493,41 +2385,47 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="7" t="s">
-        <v>0</v>
+    <row r="75" spans="1:7">
+      <c r="A75" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="B75" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C75" t="s">
         <v>82</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="7" t="s">
-        <v>33</v>
+      <c r="D75" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="B76" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C76" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" hidden="1">
+        <v>54</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F76" t="s">
+        <v>110</v>
+      </c>
+      <c r="G76" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" hidden="1">
       <c r="A77" s="5" t="s">
         <v>106</v>
       </c>
@@ -2541,60 +2439,69 @@
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:7">
       <c r="A78" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C78" t="s">
         <v>82</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="D78" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E78" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="7" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C79" t="s">
         <v>82</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>54</v>
+      <c r="D79" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="E79" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="7" t="s">
-        <v>20</v>
+      <c r="F79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C80" t="s">
         <v>82</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E80" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80" t="s">
+        <v>110</v>
+      </c>
+      <c r="G80" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="7" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>54</v>
@@ -2602,84 +2509,90 @@
       <c r="C81" t="s">
         <v>82</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="D81" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" t="s">
+        <v>47</v>
+      </c>
+      <c r="F81" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B82" t="s">
+        <v>29</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C82" t="s">
-        <v>83</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+        <v>82</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" t="s">
+        <v>43</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C83" t="s">
         <v>82</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E83" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="D83" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B84" t="s">
-        <v>47</v>
+        <v>61</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C84" t="s">
         <v>82</v>
       </c>
-      <c r="D84" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="3" t="s">
-        <v>21</v>
+      <c r="D84" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E84" t="s">
+        <v>54</v>
+      </c>
+      <c r="F84" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C85" t="s">
         <v>82</v>
       </c>
-      <c r="D85" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="3" t="s">
-        <v>49</v>
+      <c r="D85" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E85" t="s">
+        <v>47</v>
+      </c>
+      <c r="F85" t="s">
+        <v>110</v>
+      </c>
+      <c r="G85" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="B86" t="s">
         <v>54</v>
@@ -2687,18 +2600,21 @@
       <c r="C86" t="s">
         <v>82</v>
       </c>
-      <c r="D86" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B87" s="3" t="s">
+      <c r="D86" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E86" t="s">
+        <v>47</v>
+      </c>
+      <c r="F86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B87" t="s">
         <v>54</v>
       </c>
       <c r="C87" t="s">
@@ -2710,25 +2626,31 @@
       <c r="E87" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="1" t="s">
-        <v>100</v>
+      <c r="F87" t="s">
+        <v>110</v>
+      </c>
+      <c r="G87" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B88" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C88" t="s">
         <v>82</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E88" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" hidden="1">
+        <v>47</v>
+      </c>
+      <c r="F88" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" hidden="1">
       <c r="A89" s="3" t="s">
         <v>79</v>
       </c>
@@ -2740,7 +2662,7 @@
       </c>
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:5" hidden="1">
+    <row r="90" spans="1:7" hidden="1">
       <c r="A90" s="3" t="s">
         <v>79</v>
       </c>
@@ -2752,7 +2674,7 @@
       </c>
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:5" hidden="1">
+    <row r="91" spans="1:7" hidden="1">
       <c r="A91" s="3" t="s">
         <v>76</v>
       </c>
@@ -2764,9 +2686,9 @@
       </c>
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:7">
       <c r="A92" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B92" t="s">
         <v>47</v>
@@ -2774,14 +2696,17 @@
       <c r="C92" t="s">
         <v>82</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E92" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" hidden="1">
+      <c r="D92" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F92" t="s">
+        <v>146</v>
+      </c>
+      <c r="G92" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" hidden="1">
       <c r="A93" s="3" t="s">
         <v>70</v>
       </c>
@@ -2793,7 +2718,7 @@
       </c>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:5" hidden="1">
+    <row r="94" spans="1:7" hidden="1">
       <c r="A94" s="3" t="s">
         <v>71</v>
       </c>
@@ -2805,7 +2730,7 @@
       </c>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:5" hidden="1">
+    <row r="95" spans="1:7" hidden="1">
       <c r="A95" s="3" t="s">
         <v>72</v>
       </c>
@@ -2817,80 +2742,71 @@
       </c>
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="1:5">
-      <c r="A96" s="6" t="s">
-        <v>101</v>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>71</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C96" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E96" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:7">
-      <c r="A97" s="3" t="s">
-        <v>60</v>
+      <c r="A97" t="s">
+        <v>72</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C97" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E97" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B98" t="s">
-        <v>54</v>
+        <v>31</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C98" t="s">
         <v>82</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E98" t="s">
-        <v>54</v>
-      </c>
-      <c r="G98" t="s">
-        <v>149</v>
+      <c r="D98" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B99" t="s">
+        <v>62</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C99" t="s">
         <v>82</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E99" t="s">
-        <v>54</v>
+      <c r="D99" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:7">
-      <c r="A100" s="3" t="s">
-        <v>3</v>
+      <c r="A100" t="s">
+        <v>45</v>
       </c>
       <c r="B100" t="s">
         <v>47</v>
@@ -2898,36 +2814,36 @@
       <c r="C100" t="s">
         <v>82</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E100" s="3" t="s">
+      <c r="D100" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="101" spans="1:7">
-      <c r="A101" s="3" t="s">
-        <v>11</v>
+      <c r="A101" t="s">
+        <v>142</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C101" t="s">
         <v>82</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="E101" t="s">
+        <v>47</v>
+      </c>
+      <c r="F101" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:7">
-      <c r="A102" s="3" t="s">
-        <v>37</v>
+      <c r="A102" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C102" t="s">
         <v>82</v>
@@ -2938,38 +2854,52 @@
       <c r="E102" t="s">
         <v>47</v>
       </c>
+      <c r="F102" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="103" spans="1:7">
-      <c r="A103" s="3" t="s">
-        <v>22</v>
+      <c r="A103" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C103" t="s">
         <v>82</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E103" t="s">
         <v>47</v>
       </c>
+      <c r="F103" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="104" spans="1:7">
-      <c r="A104" s="3" t="s">
-        <v>27</v>
+      <c r="A104" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C104" t="s">
         <v>82</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E104" s="3"/>
+      <c r="D104" t="s">
+        <v>54</v>
+      </c>
+      <c r="E104" t="s">
+        <v>47</v>
+      </c>
+      <c r="F104" t="s">
+        <v>110</v>
+      </c>
+      <c r="G104" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="105" spans="1:7" hidden="1">
       <c r="A105" s="3" t="s">
@@ -2984,10 +2914,10 @@
       <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:7">
-      <c r="A106" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B106" s="3" t="s">
+      <c r="A106" t="s">
+        <v>25</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C106" t="s">
@@ -2996,88 +2926,107 @@
       <c r="D106" t="s">
         <v>47</v>
       </c>
-      <c r="E106" s="3"/>
+      <c r="E106" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="3" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C107" t="s">
         <v>82</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E107" s="3"/>
+      <c r="D107" t="s">
+        <v>54</v>
+      </c>
+      <c r="E107" t="s">
+        <v>54</v>
+      </c>
+      <c r="F107" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B108" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
         <v>47</v>
       </c>
       <c r="C108" t="s">
         <v>82</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>47</v>
+      <c r="D108" t="s">
+        <v>47</v>
+      </c>
+      <c r="E108" t="s">
+        <v>47</v>
+      </c>
+      <c r="F108" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="109" spans="1:7">
-      <c r="A109" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>47</v>
+      <c r="A109" t="s">
+        <v>39</v>
+      </c>
+      <c r="B109" t="s">
+        <v>54</v>
       </c>
       <c r="C109" t="s">
         <v>82</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>47</v>
+      <c r="D109" t="s">
+        <v>47</v>
+      </c>
+      <c r="E109" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="110" spans="1:7">
-      <c r="A110" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C110" t="s">
-        <v>82</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>54</v>
+      <c r="A110" t="s">
+        <v>138</v>
+      </c>
+      <c r="B110" t="s">
+        <v>54</v>
+      </c>
+      <c r="D110" t="s">
+        <v>47</v>
       </c>
       <c r="E110" t="s">
         <v>47</v>
+      </c>
+      <c r="F110" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B111" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B111" t="s">
         <v>47</v>
       </c>
       <c r="C111" t="s">
         <v>82</v>
       </c>
-      <c r="D111" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>47</v>
+      <c r="D111" t="s">
+        <v>47</v>
+      </c>
+      <c r="E111" t="s">
+        <v>47</v>
+      </c>
+      <c r="F111" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="112" spans="1:7">
-      <c r="A112" s="1" t="s">
-        <v>110</v>
+      <c r="A112" t="s">
+        <v>137</v>
       </c>
       <c r="B112" t="s">
         <v>54</v>
@@ -3085,31 +3034,37 @@
       <c r="C112" t="s">
         <v>82</v>
       </c>
-      <c r="D112" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
-      <c r="A113" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B113" s="3" t="s">
+      <c r="D112" t="s">
+        <v>47</v>
+      </c>
+      <c r="E112" t="s">
+        <v>54</v>
+      </c>
+      <c r="F112" t="s">
+        <v>146</v>
+      </c>
+      <c r="G112" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>17</v>
+      </c>
+      <c r="B113" t="s">
         <v>47</v>
       </c>
       <c r="C113" t="s">
         <v>82</v>
       </c>
-      <c r="D113" s="6" t="s">
+      <c r="D113" t="s">
         <v>47</v>
       </c>
       <c r="E113" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1">
+    <row r="114" spans="1:7" hidden="1">
       <c r="A114" s="3" t="s">
         <v>65</v>
       </c>
@@ -3123,7 +3078,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1">
+    <row r="115" spans="1:7" hidden="1">
       <c r="A115" s="3" t="s">
         <v>81</v>
       </c>
@@ -3138,21 +3093,27 @@
         <v>54</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
-      <c r="A116" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>47</v>
+    <row r="116" spans="1:7">
+      <c r="A116" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B116" t="s">
+        <v>54</v>
       </c>
       <c r="C116" t="s">
         <v>82</v>
       </c>
-      <c r="D116" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" hidden="1">
+      <c r="D116" t="s">
+        <v>54</v>
+      </c>
+      <c r="E116" t="s">
+        <v>54</v>
+      </c>
+      <c r="F116" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" hidden="1">
       <c r="A117" s="3" t="s">
         <v>77</v>
       </c>
@@ -3164,21 +3125,24 @@
       </c>
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B118" s="3" t="s">
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" t="s">
         <v>47</v>
       </c>
       <c r="C118" t="s">
         <v>82</v>
       </c>
-      <c r="D118" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" hidden="1">
+      <c r="D118" t="s">
+        <v>47</v>
+      </c>
+      <c r="E118" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" hidden="1">
       <c r="A119" s="3" t="s">
         <v>67</v>
       </c>
@@ -3190,85 +3154,98 @@
       </c>
       <c r="D119" s="3"/>
     </row>
-    <row r="120" spans="1:5">
-      <c r="A120" t="s">
-        <v>71</v>
-      </c>
-      <c r="B120" s="3" t="s">
+    <row r="120" spans="1:7">
+      <c r="A120" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" t="s">
         <v>54</v>
       </c>
       <c r="C120" t="s">
-        <v>143</v>
-      </c>
-      <c r="D120" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D120" t="s">
         <v>54</v>
       </c>
       <c r="E120" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>72</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>54</v>
+        <v>19</v>
+      </c>
+      <c r="B121" t="s">
+        <v>47</v>
       </c>
       <c r="C121" t="s">
-        <v>143</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>54</v>
+        <v>82</v>
+      </c>
+      <c r="D121" t="s">
+        <v>47</v>
       </c>
       <c r="E121" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
-      <c r="A122" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>47</v>
+    <row r="122" spans="1:7">
+      <c r="A122" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>54</v>
       </c>
       <c r="C122" t="s">
         <v>82</v>
       </c>
-      <c r="D122" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="D122" t="s">
+        <v>54</v>
+      </c>
+      <c r="E122" t="s">
+        <v>47</v>
+      </c>
+      <c r="F122" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
       <c r="A123" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C123" t="s">
-        <v>82</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
-      <c r="A124" t="s">
-        <v>45</v>
+        <v>121</v>
+      </c>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C124" t="s">
         <v>82</v>
       </c>
-      <c r="D124" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="D124" t="s">
+        <v>54</v>
+      </c>
+      <c r="E124" t="s">
+        <v>47</v>
+      </c>
+      <c r="F124" t="s">
+        <v>110</v>
+      </c>
+      <c r="G124" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>47</v>
@@ -3283,29 +3260,29 @@
         <v>47</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
-      <c r="A126" t="s">
-        <v>39</v>
-      </c>
-      <c r="B126" t="s">
+    <row r="126" spans="1:7">
+      <c r="A126" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B126" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C126" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D126" t="s">
         <v>47</v>
       </c>
       <c r="E126" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="B127" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C127" t="s">
         <v>82</v>
@@ -3314,12 +3291,15 @@
         <v>47</v>
       </c>
       <c r="E127" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5">
+        <v>54</v>
+      </c>
+      <c r="F127" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B128" t="s">
         <v>47</v>
@@ -3334,77 +3314,86 @@
         <v>47</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
-      <c r="A129" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B129" t="s">
-        <v>54</v>
-      </c>
-      <c r="C129" t="s">
-        <v>82</v>
-      </c>
-      <c r="D129" t="s">
-        <v>54</v>
+    <row r="129" spans="1:6">
+      <c r="A129" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E129" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
-      <c r="A130" t="s">
-        <v>19</v>
+    <row r="130" spans="1:6">
+      <c r="A130" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="B130" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C130" t="s">
         <v>82</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E130" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
-      <c r="A131" t="s">
-        <v>26</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>47</v>
+      <c r="F130" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B131" t="s">
+        <v>54</v>
       </c>
       <c r="C131" t="s">
         <v>82</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E131" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>54</v>
+        <v>16</v>
+      </c>
+      <c r="B132" t="s">
+        <v>47</v>
       </c>
       <c r="C132" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D132" t="s">
         <v>47</v>
       </c>
       <c r="E132" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
+        <v>151</v>
+      </c>
+      <c r="F132" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B133" t="s">
         <v>47</v>
@@ -3416,24 +3405,30 @@
         <v>47</v>
       </c>
       <c r="E133" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
+        <v>54</v>
+      </c>
+      <c r="F133" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="C134" t="s">
+        <v>82</v>
+      </c>
+      <c r="D134" t="s">
+        <v>54</v>
       </c>
       <c r="E134" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="F134" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>